<commit_message>
Fixed Superbowl not lining up with right year
</commit_message>
<xml_diff>
--- a/NFL Excel Sheets/Defense_RECEIVING.xlsx
+++ b/NFL Excel Sheets/Defense_RECEIVING.xlsx
@@ -40869,12 +40869,12 @@
       </c>
       <c r="D1447" t="inlineStr">
         <is>
-          <t>2,689</t>
+          <t>3,471</t>
         </is>
       </c>
       <c r="E1447" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1447" t="n">
@@ -40892,17 +40892,17 @@
       </c>
       <c r="C1448" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Minnesota Vikings</t>
         </is>
       </c>
       <c r="D1448" t="inlineStr">
         <is>
-          <t>2,656</t>
+          <t>2,924</t>
         </is>
       </c>
       <c r="E1448" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1448" t="n">
@@ -40920,17 +40920,17 @@
       </c>
       <c r="C1449" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="D1449" t="inlineStr">
         <is>
-          <t>2,605</t>
+          <t>3,020</t>
         </is>
       </c>
       <c r="E1449" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F1449" t="n">
@@ -40948,17 +40948,17 @@
       </c>
       <c r="C1450" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
       <c r="D1450" t="inlineStr">
         <is>
-          <t>2,249</t>
+          <t>3,073</t>
         </is>
       </c>
       <c r="E1450" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1450" t="n">
@@ -40976,17 +40976,17 @@
       </c>
       <c r="C1451" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>Indianapolis Colts</t>
         </is>
       </c>
       <c r="D1451" t="inlineStr">
         <is>
-          <t>2,495</t>
+          <t>2,737</t>
         </is>
       </c>
       <c r="E1451" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1451" t="n">
@@ -41004,17 +41004,17 @@
       </c>
       <c r="C1452" t="inlineStr">
         <is>
-          <t>Washington Redskins</t>
+          <t>Seattle Seahawks</t>
         </is>
       </c>
       <c r="D1452" t="inlineStr">
         <is>
-          <t>2,199</t>
+          <t>2,853</t>
         </is>
       </c>
       <c r="E1452" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1452" t="n">
@@ -41037,7 +41037,7 @@
       </c>
       <c r="D1453" t="inlineStr">
         <is>
-          <t>2,275</t>
+          <t>2,809</t>
         </is>
       </c>
       <c r="E1453" t="inlineStr">
@@ -41065,12 +41065,12 @@
       </c>
       <c r="D1454" t="inlineStr">
         <is>
-          <t>2,010</t>
+          <t>2,452</t>
         </is>
       </c>
       <c r="E1454" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F1454" t="n">
@@ -41088,17 +41088,17 @@
       </c>
       <c r="C1455" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>New York Jets</t>
         </is>
       </c>
       <c r="D1455" t="inlineStr">
         <is>
-          <t>2,290</t>
+          <t>2,704</t>
         </is>
       </c>
       <c r="E1455" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1455" t="n">
@@ -41116,12 +41116,12 @@
       </c>
       <c r="C1456" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Atlanta Falcons</t>
         </is>
       </c>
       <c r="D1456" t="inlineStr">
         <is>
-          <t>2,525</t>
+          <t>2,758</t>
         </is>
       </c>
       <c r="E1456" t="inlineStr">
@@ -41144,12 +41144,12 @@
       </c>
       <c r="C1457" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>Tennessee Titans</t>
         </is>
       </c>
       <c r="D1457" t="inlineStr">
         <is>
-          <t>2,182</t>
+          <t>2,736</t>
         </is>
       </c>
       <c r="E1457" t="inlineStr">
@@ -41172,17 +41172,17 @@
       </c>
       <c r="C1458" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Detroit Lions</t>
         </is>
       </c>
       <c r="D1458" t="inlineStr">
         <is>
-          <t>2,309</t>
+          <t>3,024</t>
         </is>
       </c>
       <c r="E1458" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F1458" t="n">
@@ -41200,17 +41200,17 @@
       </c>
       <c r="C1459" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>Los Angeles Rams</t>
         </is>
       </c>
       <c r="D1459" t="inlineStr">
         <is>
-          <t>2,260</t>
+          <t>2,527</t>
         </is>
       </c>
       <c r="E1459" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F1459" t="n">
@@ -41233,7 +41233,7 @@
       </c>
       <c r="D1460" t="inlineStr">
         <is>
-          <t>2,007</t>
+          <t>2,554</t>
         </is>
       </c>
       <c r="E1460" t="inlineStr">
@@ -41256,12 +41256,12 @@
       </c>
       <c r="C1461" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>Dallas Cowboys</t>
         </is>
       </c>
       <c r="D1461" t="inlineStr">
         <is>
-          <t>2,449</t>
+          <t>2,372</t>
         </is>
       </c>
       <c r="E1461" t="inlineStr">
@@ -41279,17 +41279,17 @@
       </c>
       <c r="B1462" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C1462" t="inlineStr">
         <is>
-          <t>Oakland Raiders</t>
+          <t>New Orleans Saints</t>
         </is>
       </c>
       <c r="D1462" t="inlineStr">
         <is>
-          <t>2,495</t>
+          <t>2,513</t>
         </is>
       </c>
       <c r="E1462" t="inlineStr">
@@ -41307,17 +41307,17 @@
       </c>
       <c r="B1463" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C1463" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Washington Redskins</t>
         </is>
       </c>
       <c r="D1463" t="inlineStr">
         <is>
-          <t>1,943</t>
+          <t>2,492</t>
         </is>
       </c>
       <c r="E1463" t="inlineStr">
@@ -41335,22 +41335,22 @@
       </c>
       <c r="B1464" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C1464" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>Los Angeles Chargers</t>
         </is>
       </c>
       <c r="D1464" t="inlineStr">
         <is>
-          <t>2,407</t>
+          <t>2,417</t>
         </is>
       </c>
       <c r="E1464" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F1464" t="n">
@@ -41363,22 +41363,22 @@
       </c>
       <c r="B1465" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C1465" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Pittsburgh Steelers</t>
         </is>
       </c>
       <c r="D1465" t="inlineStr">
         <is>
-          <t>1,913</t>
+          <t>2,455</t>
         </is>
       </c>
       <c r="E1465" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1465" t="n">
@@ -41396,17 +41396,17 @@
       </c>
       <c r="C1466" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Oakland Raiders</t>
         </is>
       </c>
       <c r="D1466" t="inlineStr">
         <is>
-          <t>2,086</t>
+          <t>2,817</t>
         </is>
       </c>
       <c r="E1466" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F1466" t="n">
@@ -41419,22 +41419,22 @@
       </c>
       <c r="B1467" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C1467" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Philadelphia Eagles</t>
         </is>
       </c>
       <c r="D1467" t="inlineStr">
         <is>
-          <t>1,974</t>
+          <t>2,540</t>
         </is>
       </c>
       <c r="E1467" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F1467" t="n">
@@ -41447,22 +41447,22 @@
       </c>
       <c r="B1468" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C1468" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Buffalo Bills</t>
         </is>
       </c>
       <c r="D1468" t="inlineStr">
         <is>
-          <t>2,019</t>
+          <t>2,167</t>
         </is>
       </c>
       <c r="E1468" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F1468" t="n">
@@ -41475,22 +41475,22 @@
       </c>
       <c r="B1469" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C1469" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Green Bay Packers</t>
         </is>
       </c>
       <c r="D1469" t="inlineStr">
         <is>
-          <t>2,017</t>
+          <t>2,756</t>
         </is>
       </c>
       <c r="E1469" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1469" t="n">
@@ -41508,17 +41508,17 @@
       </c>
       <c r="C1470" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>Denver Broncos</t>
         </is>
       </c>
       <c r="D1470" t="inlineStr">
         <is>
-          <t>2,219</t>
+          <t>2,232</t>
         </is>
       </c>
       <c r="E1470" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1470" t="n">
@@ -41536,17 +41536,17 @@
       </c>
       <c r="C1471" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>New York Giants</t>
         </is>
       </c>
       <c r="D1471" t="inlineStr">
         <is>
-          <t>2,018</t>
+          <t>2,755</t>
         </is>
       </c>
       <c r="E1471" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1471" t="n">
@@ -41564,17 +41564,17 @@
       </c>
       <c r="C1472" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Baltimore Ravens</t>
         </is>
       </c>
       <c r="D1472" t="inlineStr">
         <is>
-          <t>2,129</t>
+          <t>2,555</t>
         </is>
       </c>
       <c r="E1472" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F1472" t="n">
@@ -41592,17 +41592,17 @@
       </c>
       <c r="C1473" t="inlineStr">
         <is>
-          <t>Miami Dolphins</t>
+          <t>Jacksonville Jaguars</t>
         </is>
       </c>
       <c r="D1473" t="inlineStr">
         <is>
-          <t>2,085</t>
+          <t>2,408</t>
         </is>
       </c>
       <c r="E1473" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1473" t="n">
@@ -41620,17 +41620,17 @@
       </c>
       <c r="C1474" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>Cleveland Browns</t>
         </is>
       </c>
       <c r="D1474" t="inlineStr">
         <is>
-          <t>1,606</t>
+          <t>2,379</t>
         </is>
       </c>
       <c r="E1474" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1474" t="n">
@@ -41643,22 +41643,22 @@
       </c>
       <c r="B1475" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C1475" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>Miami Dolphins</t>
         </is>
       </c>
       <c r="D1475" t="inlineStr">
         <is>
-          <t>1,892</t>
+          <t>2,545</t>
         </is>
       </c>
       <c r="E1475" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F1475" t="n">
@@ -41671,22 +41671,22 @@
       </c>
       <c r="B1476" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C1476" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Cincinnati Bengals</t>
         </is>
       </c>
       <c r="D1476" t="inlineStr">
         <is>
-          <t>1,566</t>
+          <t>2,661</t>
         </is>
       </c>
       <c r="E1476" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F1476" t="n">
@@ -41704,17 +41704,17 @@
       </c>
       <c r="C1477" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>New England Patriots</t>
         </is>
       </c>
       <c r="D1477" t="inlineStr">
         <is>
-          <t>2,126</t>
+          <t>1,780</t>
         </is>
       </c>
       <c r="E1477" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F1477" t="n">
@@ -41737,12 +41737,12 @@
       </c>
       <c r="D1478" t="inlineStr">
         <is>
-          <t>1,353</t>
+          <t>1,735</t>
         </is>
       </c>
       <c r="E1478" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F1478" t="n">

</xml_diff>